<commit_message>
Append some level 2 notes.
</commit_message>
<xml_diff>
--- a/Notes/Levels.xlsx
+++ b/Notes/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PersonalFiles\Project\Kylin\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D2EE69-1C0F-4F73-960D-AEFAE9D6F3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9032006B-9AFB-4785-9BF8-7BB5120066A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11496" yWindow="168" windowWidth="20160" windowHeight="11844" xr2:uid="{E0EB0FAE-C925-4820-8CD5-D084D1F160F4}"/>
+    <workbookView xWindow="5256" yWindow="3012" windowWidth="20160" windowHeight="11844" xr2:uid="{E0EB0FAE-C925-4820-8CD5-D084D1F160F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>个人攻击，一般灾害，恢复部分功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -206,6 +206,26 @@
   </si>
   <si>
     <t>安全审计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+根据会话状态信息，为进出数据流提供明确的允许、拒绝访问能力。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键网络节点监视网络攻击行为。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键网络节点对恶意代码进行检测和清除，并维护恶意代码防护机制的升级和更新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>划分不同的网络区域，并按照方便管理控制原则分配地址，避免将重要网络部署于边界，采用可靠技术手段隔离其他网络区域。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络边界和重要网络节点进行安全审计、审计覆盖每个用户，对重要的用户行为和安全事件进行审计；审计记录包括事件时间、用户、事件类型、时间是否成功与其他审计相关信息；对审计记录进行保护、定期备份，避免受到未预期的删除、修改或覆盖等。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -588,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8BD1EC-8069-49D4-BDE4-919DE465E619}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -676,8 +696,8 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -711,7 +731,9 @@
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -722,7 +744,9 @@
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -825,25 +849,29 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update protect 2, create protect 3.
</commit_message>
<xml_diff>
--- a/Notes/Levels.xlsx
+++ b/Notes/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PersonalFiles\Project\Kylin\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9032006B-9AFB-4785-9BF8-7BB5120066A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F967C4ED-0875-4E57-B9F4-478123A04693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="3012" windowWidth="20160" windowHeight="11844" xr2:uid="{E0EB0FAE-C925-4820-8CD5-D084D1F160F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27096" windowHeight="16416" xr2:uid="{E0EB0FAE-C925-4820-8CD5-D084D1F160F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>个人攻击，一般灾害，恢复部分功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,11 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>对登录的用户身份进行标识鉴别，身份具有唯一
-性，需要有复杂度并定期更换。需要处理登录失败，结束会话、限制非法登录次数、超时自动退出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户访问控制</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,9 +95,6 @@
   <si>
     <t>入侵防范</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小安装原则、仅安装需要的组件和应用程序，关闭不需要的系统服务、默认共享和高危端口</t>
   </si>
   <si>
     <t>恶意代码防范</t>
@@ -213,19 +205,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>关键网络节点监视网络攻击行为。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关键网络节点对恶意代码进行检测和清除，并维护恶意代码防护机制的升级和更新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>划分不同的网络区域，并按照方便管理控制原则分配地址，避免将重要网络部署于边界，采用可靠技术手段隔离其他网络区域。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>网络边界和重要网络节点进行安全审计、审计覆盖每个用户，对重要的用户行为和安全事件进行审计；审计记录包括事件时间、用户、事件类型、时间是否成功与其他审计相关信息；对审计记录进行保护、定期备份，避免受到未预期的删除、修改或覆盖等。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+应授予管理用户所需的最小权限，实现管理用户的权限分离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键网络节点对恶意代码进行检测和清除，并维护恶意代码防护机制的升级和更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+当进行远程管理时，应对采用必要措施防止鉴别信息在网络传输过程中被窃听</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对登录的用户身份进行标识鉴别，身份具有唯一性，需要有复杂度并定期更换。需要处理登录失败，结束会话、限制非法登录次数、超时自动退出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小安装原则、仅安装需要的组件和应用程序，关闭不需要的系统服务、默认共享和高危端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+关键网络节点监视网络攻击行为。通过设定终端接入方式或网络地址范围对网络进行管理的中断进行限制。提供数据有效性验证功能，保证通过人机接口输入或通过通信接口输入的内容符合系统设定要求。应能发现可存在的已知漏洞，经过充分测试评估后及时修补漏洞。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -608,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8BD1EC-8069-49D4-BDE4-919DE465E619}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -668,10 +676,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -697,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -707,42 +715,46 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>46</v>
@@ -752,10 +764,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -763,10 +775,10 @@
     </row>
     <row r="12" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -774,10 +786,10 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -785,10 +797,10 @@
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -796,10 +808,10 @@
     </row>
     <row r="15" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -807,10 +819,10 @@
     </row>
     <row r="16" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -818,10 +830,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -829,10 +841,10 @@
     </row>
     <row r="18" spans="1:5" ht="69" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -840,10 +852,10 @@
     </row>
     <row r="19" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -851,26 +863,26 @@
     </row>
     <row r="20" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>

</xml_diff>